<commit_message>
Refactor profit computation and electricity price extraction
</commit_message>
<xml_diff>
--- a/data/37-intersection map Aggregator Competition.xlsx
+++ b/data/37-intersection map Aggregator Competition.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Documents\GitHub\TFM-EV-Routing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002D8DBF-6C13-45C9-88B8-57510A8C725E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FCB2E0-BB65-4B93-B032-AB8B12E91657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sChargingStations" sheetId="5" r:id="rId1"/>
-    <sheet name="sTimePeriods" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>pStationIntersection</t>
   </si>
@@ -45,15 +44,6 @@
     <t>pMaxChargingPrice [$/kWh]</t>
   </si>
   <si>
-    <t>pPeriod</t>
-  </si>
-  <si>
-    <t>pElectricityCost [$/kWh]</t>
-  </si>
-  <si>
-    <t>aux_pElectricityCost [€/MWh]</t>
-  </si>
-  <si>
     <t>pChargingPrice [$/kWh]</t>
   </si>
 </sst>
@@ -61,9 +51,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,13 +107,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,14 +396,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -433,17 +418,17 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>11</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.8</v>
       </c>
     </row>
@@ -451,10 +436,10 @@
       <c r="A3" s="1">
         <v>14</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.8</v>
       </c>
     </row>
@@ -462,10 +447,10 @@
       <c r="A4" s="1">
         <v>15</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.8</v>
       </c>
     </row>
@@ -473,7 +458,7 @@
       <c r="A5" s="1">
         <v>26</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>0.6</v>
       </c>
     </row>
@@ -481,327 +466,8 @@
       <c r="A6" s="1">
         <v>37</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75461178-76FA-4772-B068-DC79A26BB340}">
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>19.12</v>
-      </c>
-      <c r="C2" s="5">
-        <f>B2*0.00142</f>
-        <v>2.7150400000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>28.68</v>
-      </c>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C24" si="0">B3*0.00142</f>
-        <v>4.0725600000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>23.6</v>
-      </c>
-      <c r="C4" s="5">
-        <f t="shared" si="0"/>
-        <v>3.3512E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>22.85</v>
-      </c>
-      <c r="C5" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2447000000000004E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>24.24</v>
-      </c>
-      <c r="C6" s="5">
-        <f t="shared" si="0"/>
-        <v>3.4420800000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>26.15</v>
-      </c>
-      <c r="C7" s="5">
-        <f t="shared" si="0"/>
-        <v>3.7132999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>27.95</v>
-      </c>
-      <c r="C8" s="5">
-        <f t="shared" si="0"/>
-        <v>3.9689000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3">
-        <v>36.909999999999997</v>
-      </c>
-      <c r="C9" s="5">
-        <f t="shared" si="0"/>
-        <v>5.2412199999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3">
-        <v>49.89</v>
-      </c>
-      <c r="C10" s="5">
-        <f t="shared" si="0"/>
-        <v>7.0843799999999998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <v>53.1</v>
-      </c>
-      <c r="C11" s="5">
-        <f t="shared" si="0"/>
-        <v>7.5402000000000011E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3">
-        <v>28.39</v>
-      </c>
-      <c r="C12" s="5">
-        <f t="shared" si="0"/>
-        <v>4.0313800000000004E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3">
-        <v>13.28</v>
-      </c>
-      <c r="C13" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8857599999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>12.23</v>
-      </c>
-      <c r="C14" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7366599999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <v>11.97</v>
-      </c>
-      <c r="C15" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6997400000000003E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3">
-        <v>12.46</v>
-      </c>
-      <c r="C16" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7693200000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3">
-        <v>10.58</v>
-      </c>
-      <c r="C17" s="5">
-        <f t="shared" si="0"/>
-        <v>1.50236E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>9.27</v>
-      </c>
-      <c r="C18" s="5">
-        <f t="shared" si="0"/>
-        <v>1.31634E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3">
-        <v>9.93</v>
-      </c>
-      <c r="C19" s="5">
-        <f t="shared" si="0"/>
-        <v>1.41006E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="C20" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1658200000000002E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3">
-        <v>10.36</v>
-      </c>
-      <c r="C21" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4711199999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3">
-        <v>13.76</v>
-      </c>
-      <c r="C22" s="5">
-        <f t="shared" si="0"/>
-        <v>1.95392E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3">
-        <v>43.83</v>
-      </c>
-      <c r="C23" s="5">
-        <f t="shared" si="0"/>
-        <v>6.2238599999999998E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3">
-        <v>48.02</v>
-      </c>
-      <c r="C24" s="5">
-        <f t="shared" si="0"/>
-        <v>6.818840000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3">
-        <v>32</v>
-      </c>
-      <c r="C25" s="5">
-        <f>B25*0.00142</f>
-        <v>4.5440000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>